<commit_message>
Updated Sprint-3 files on drive copied to Git versioning. (not written by just me)
</commit_message>
<xml_diff>
--- a/Sprint_3/Requirement_ID-Table_v2.xlsx
+++ b/Sprint_3/Requirement_ID-Table_v2.xlsx
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -240,19 +240,28 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -567,7 +576,7 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -581,7 +590,7 @@
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -595,7 +604,7 @@
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -609,7 +618,7 @@
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -623,7 +632,7 @@
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -637,7 +646,7 @@
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -651,7 +660,7 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -665,7 +674,7 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -679,7 +688,7 @@
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -693,7 +702,7 @@
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -707,7 +716,7 @@
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -721,7 +730,7 @@
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -735,7 +744,7 @@
       <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -749,7 +758,7 @@
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -757,86 +766,86 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>